<commit_message>
Mise à jour de la répartition des gains
</commit_message>
<xml_diff>
--- a/public/assets/Répartition des gains.xlsx
+++ b/public/assets/Répartition des gains.xlsx
@@ -60,7 +60,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -71,6 +71,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -102,27 +108,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -436,14 +448,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="2.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="7" width="25.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="9" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="9" width="8.290714285714287" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="9" width="8.005" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="10" width="5.005" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="7" width="2.005" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
@@ -453,19 +465,19 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3">
+      <c r="G1" s="4">
         <v>68.3</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -476,132 +488,132 @@
       <c r="A2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="3">
-        <f>70.5</f>
-      </c>
-      <c r="C2" s="3">
+      <c r="B2" s="4">
+        <f>86</f>
+      </c>
+      <c r="C2" s="4">
         <f>10*(B2*0.01)</f>
       </c>
-      <c r="D2" s="3">
+      <c r="D2" s="4">
         <f>30*(B2*0.01)</f>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="4">
         <f>50*(B2*0.01)</f>
       </c>
-      <c r="F2" s="3">
+      <c r="F2" s="4">
         <f>G1*(B2*0.01)</f>
       </c>
-      <c r="G2" s="4"/>
+      <c r="G2" s="5"/>
       <c r="H2" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="5">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="B3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="C3" s="4">
         <f>10*(B3*0.01)</f>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="4">
         <f>30*(B3*0.01)</f>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="6">
         <f>50*(B3*0.01)</f>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="4">
         <f>G1*(B3*0.01)</f>
       </c>
-      <c r="G3" s="4"/>
+      <c r="G3" s="5"/>
       <c r="H3" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="5">
-        <v>16</v>
-      </c>
-      <c r="C4" s="3">
+      <c r="B4" s="6">
+        <v>8</v>
+      </c>
+      <c r="C4" s="4">
         <f>10*(B4*0.01)</f>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="4">
         <f>30*(B4*0.01)</f>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="6">
         <f>50*(B4*0.01)</f>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="4">
         <f>G1*(B4*0.01)</f>
       </c>
-      <c r="G4" s="4"/>
+      <c r="G4" s="5"/>
       <c r="H4" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="3">
-        <v>3.5</v>
-      </c>
-      <c r="C5" s="3">
+      <c r="B5" s="4">
+        <v>3</v>
+      </c>
+      <c r="C5" s="4">
         <f>10*(B5*0.01)</f>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="4">
         <f>30*(B5*0.01)</f>
       </c>
-      <c r="E5" s="3">
+      <c r="E5" s="4">
         <f>50*(B5*0.01)</f>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="4">
         <f>G1*(B5*0.01)</f>
       </c>
-      <c r="G5" s="4"/>
+      <c r="G5" s="5"/>
       <c r="H5" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="5">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="B6" s="6">
+        <v>3</v>
+      </c>
+      <c r="C6" s="4">
         <f>10*(B6*0.01)</f>
       </c>
-      <c r="D6" s="3">
+      <c r="D6" s="4">
         <f>30*(B6*0.01)</f>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="6">
         <f>50*(B6*0.01)</f>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="4">
         <f>G1*(B6*0.01)</f>
       </c>
-      <c r="G6" s="4"/>
+      <c r="G6" s="5"/>
       <c r="H6" s="1"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="6">
         <f>100-(B2+B3+B4+B6+B5)</f>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="6">
         <f>10*(B7*0.01)</f>
       </c>
-      <c r="D7" s="5">
+      <c r="D7" s="6">
         <f>30*(B7*0.01)</f>
       </c>
-      <c r="E7" s="5">
+      <c r="E7" s="6">
         <f>50*(B7*0.01)</f>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="6">
         <f>G1*(B7*0.01)</f>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="5"/>
       <c r="H7" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Répartition des gains.xlsx
</commit_message>
<xml_diff>
--- a/public/assets/Répartition des gains.xlsx
+++ b/public/assets/Répartition des gains.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+  <si>
+    <t>Jeux</t>
+  </si>
   <si>
     <t>But/raison</t>
   </si>
@@ -34,9 +37,6 @@
     <t>Pour :</t>
   </si>
   <si>
-    <t>€</t>
-  </si>
-  <si>
     <t>Rémunération du créateur</t>
   </si>
   <si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Reste</t>
+  </si>
+  <si>
+    <t>Musiques</t>
+  </si>
+  <si>
+    <t>Exemple pour 0,5€</t>
   </si>
 </sst>
 </file>
@@ -69,27 +75,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Speak Pro"/>
       <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <name val="Speak Pro"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFed7d31"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFffff00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -98,34 +114,325 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFc6c6c6"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFc6c6c6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFc6c6c6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFc6c6c6"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="43">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="3" applyBorder="1" fontId="1" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="12" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="11" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="1" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="6" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="9" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="10" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="14" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="13" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -134,7 +441,7 @@
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -442,181 +749,389 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="7" width="25.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="8" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="9" width="15.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="9" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="9" width="8.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="9" width="8.005" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="10" width="5.005" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="7" width="2.005" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="39" width="25.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="40" width="10.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="41" width="16.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="41" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="41" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="41" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="42" width="9.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="39" width="14.147857142857141" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="26.25">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="6"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
+      <c r="A3" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="B3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="C3" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D3" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="E3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4">
+      <c r="F3" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="14">
         <v>68.3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H3" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="A4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="16">
+        <f>89.4</f>
+      </c>
+      <c r="C4" s="17">
+        <f>10*(B4*0.01)</f>
+      </c>
+      <c r="D4" s="16">
+        <f>30*(B4*0.01)</f>
+      </c>
+      <c r="E4" s="17">
+        <f>50*(B4*0.01)</f>
+      </c>
+      <c r="F4" s="16">
+        <f>G3*(B4*0.01)</f>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="A5" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="17">
+        <f>10*(B5*0.01)</f>
+      </c>
+      <c r="D5" s="16">
+        <f>30*(B5*0.01)</f>
+      </c>
+      <c r="E5" s="17">
+        <f>50*(B5*0.01)</f>
+      </c>
+      <c r="F5" s="16">
+        <f>G3*(B5*0.01)</f>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="A6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="16">
+        <v>9.05</v>
+      </c>
+      <c r="C6" s="17">
+        <f>10*(B6*0.01)</f>
+      </c>
+      <c r="D6" s="16">
+        <f>30*(B6*0.01)</f>
+      </c>
+      <c r="E6" s="17">
+        <f>50*(B6*0.01)</f>
+      </c>
+      <c r="F6" s="16">
+        <f>G3*(B6*0.01)</f>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="A7" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="16">
+        <v>0.55</v>
+      </c>
+      <c r="C7" s="17">
+        <f>10*(B7*0.01)</f>
+      </c>
+      <c r="D7" s="16">
+        <f>30*(B7*0.01)</f>
+      </c>
+      <c r="E7" s="17">
+        <f>50*(B7*0.01)</f>
+      </c>
+      <c r="F7" s="16">
+        <f>G3*(B7*0.01)</f>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
+      <c r="A8" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="16">
+        <v>0.5</v>
+      </c>
+      <c r="C8" s="17">
+        <f>10*(B8*0.01)</f>
+      </c>
+      <c r="D8" s="16">
+        <f>30*(B8*0.01)</f>
+      </c>
+      <c r="E8" s="17">
+        <f>50*(B8*0.01)</f>
+      </c>
+      <c r="F8" s="16">
+        <f>G3*(B8*0.01)</f>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="A9" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="20">
+        <f>100-(B4+B5+B6+B8+B7)</f>
+      </c>
+      <c r="C9" s="21">
+        <f>10*(B9*0.01)</f>
+      </c>
+      <c r="D9" s="22">
+        <f>30*(B9*0.01)</f>
+      </c>
+      <c r="E9" s="21">
+        <f>50*(B9*0.01)</f>
+      </c>
+      <c r="F9" s="22">
+        <f>G3*(B9*0.01)</f>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="23"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="23"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="18"/>
+      <c r="G11" s="18"/>
+      <c r="H11" s="23"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="26.25">
+      <c r="A12" s="24" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="25"/>
+      <c r="C12" s="26"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="20.25">
+      <c r="A13" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E13" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F13" s="31" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="1" t="s">
+      <c r="G13" s="32">
+        <v>68.3</v>
+      </c>
+      <c r="H13" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="A14" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4">
-        <f>86</f>
-      </c>
-      <c r="C2" s="4">
-        <f>10*(B2*0.01)</f>
-      </c>
-      <c r="D2" s="4">
-        <f>30*(B2*0.01)</f>
-      </c>
-      <c r="E2" s="4">
-        <f>50*(B2*0.01)</f>
-      </c>
-      <c r="F2" s="4">
-        <f>G1*(B2*0.01)</f>
-      </c>
-      <c r="G2" s="5"/>
-      <c r="H2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="1" t="s">
+      <c r="B14" s="34">
+        <f>90</f>
+      </c>
+      <c r="C14" s="35">
+        <f>0.5*(B14*0.01)</f>
+      </c>
+      <c r="D14" s="34">
+        <f>30*(B14*0.01)</f>
+      </c>
+      <c r="E14" s="35">
+        <f>50*(B14*0.01)</f>
+      </c>
+      <c r="F14" s="34">
+        <f>G13*(B14*0.01)</f>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="A15" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B15" s="34">
+        <v>1</v>
+      </c>
+      <c r="C15" s="35">
+        <f>0.5*(B15*0.01)</f>
+      </c>
+      <c r="D15" s="34">
+        <f>30*(B15*0.01)</f>
+      </c>
+      <c r="E15" s="35">
+        <f>50*(B15*0.01)</f>
+      </c>
+      <c r="F15" s="34">
+        <f>G13*(B15*0.01)</f>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="A16" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="34">
+        <v>9</v>
+      </c>
+      <c r="C16" s="35">
+        <f>10*(B16*0.01)</f>
+      </c>
+      <c r="D16" s="34">
+        <f>30*(B16*0.01)</f>
+      </c>
+      <c r="E16" s="35">
+        <f>50*(B16*0.01)</f>
+      </c>
+      <c r="F16" s="34">
+        <f>G13*(B16*0.01)</f>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="33" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="34">
         <v>0.5</v>
       </c>
-      <c r="C3" s="4">
-        <f>10*(B3*0.01)</f>
-      </c>
-      <c r="D3" s="4">
-        <f>30*(B3*0.01)</f>
-      </c>
-      <c r="E3" s="6">
-        <f>50*(B3*0.01)</f>
-      </c>
-      <c r="F3" s="4">
-        <f>G1*(B3*0.01)</f>
-      </c>
-      <c r="G3" s="5"/>
-      <c r="H3" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="6">
-        <v>8</v>
-      </c>
-      <c r="C4" s="4">
-        <f>10*(B4*0.01)</f>
-      </c>
-      <c r="D4" s="4">
-        <f>30*(B4*0.01)</f>
-      </c>
-      <c r="E4" s="6">
-        <f>50*(B4*0.01)</f>
-      </c>
-      <c r="F4" s="4">
-        <f>G1*(B4*0.01)</f>
-      </c>
-      <c r="G4" s="5"/>
-      <c r="H4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="4">
-        <v>3</v>
-      </c>
-      <c r="C5" s="4">
-        <f>10*(B5*0.01)</f>
-      </c>
-      <c r="D5" s="4">
-        <f>30*(B5*0.01)</f>
-      </c>
-      <c r="E5" s="4">
-        <f>50*(B5*0.01)</f>
-      </c>
-      <c r="F5" s="4">
-        <f>G1*(B5*0.01)</f>
-      </c>
-      <c r="G5" s="5"/>
-      <c r="H5" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="6">
-        <v>3</v>
-      </c>
-      <c r="C6" s="4">
-        <f>10*(B6*0.01)</f>
-      </c>
-      <c r="D6" s="4">
-        <f>30*(B6*0.01)</f>
-      </c>
-      <c r="E6" s="6">
-        <f>50*(B6*0.01)</f>
-      </c>
-      <c r="F6" s="4">
-        <f>G1*(B6*0.01)</f>
-      </c>
-      <c r="G6" s="5"/>
-      <c r="H6" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="6">
-        <f>100-(B2+B3+B4+B6+B5)</f>
-      </c>
-      <c r="C7" s="6">
-        <f>10*(B7*0.01)</f>
-      </c>
-      <c r="D7" s="6">
-        <f>30*(B7*0.01)</f>
-      </c>
-      <c r="E7" s="6">
-        <f>50*(B7*0.01)</f>
-      </c>
-      <c r="F7" s="6">
-        <f>G1*(B7*0.01)</f>
-      </c>
-      <c r="G7" s="5"/>
-      <c r="H7" s="1"/>
+      <c r="C17" s="35">
+        <f>10*(B19*0.01)</f>
+      </c>
+      <c r="D17" s="34">
+        <f>30*(B17*0.01)</f>
+      </c>
+      <c r="E17" s="35">
+        <f>50*(B17*0.01)</f>
+      </c>
+      <c r="F17" s="34">
+        <f>G13*(B17*0.01)</f>
+      </c>
+      <c r="G17" s="4"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5">
+      <c r="A18" s="33"/>
+      <c r="B18" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="C18" s="35">
+        <f>10*(B20*0.01)</f>
+      </c>
+      <c r="D18" s="34">
+        <f>30*(B18*0.01)</f>
+      </c>
+      <c r="E18" s="35">
+        <f>50*(B18*0.01)</f>
+      </c>
+      <c r="F18" s="34">
+        <f>G13*(B18*0.01)</f>
+      </c>
+      <c r="G18" s="4"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5">
+      <c r="A19" s="33"/>
+      <c r="B19" s="36">
+        <f>100-(B14+B15+B16+B18+B17)</f>
+      </c>
+      <c r="C19" s="37">
+        <f>10*(B21*0.01)</f>
+      </c>
+      <c r="D19" s="38">
+        <f>30*(B19*0.01)</f>
+      </c>
+      <c r="E19" s="37">
+        <f>50*(B19*0.01)</f>
+      </c>
+      <c r="F19" s="38">
+        <f>G13*(B19*0.01)</f>
+      </c>
+      <c r="G19" s="4"/>
+      <c r="H19" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A12:G12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>